<commit_message>
using 2 calculators example
</commit_message>
<xml_diff>
--- a/test scenarios + cases.xlsx
+++ b/test scenarios + cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qpr-my.sharepoint.com/personal/youssef_zerkani_qpr_com/Documents/Documents/NeoMore/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qpr-my.sharepoint.com/personal/youssef_zerkani_qpr_com/Documents/Documents/NeoMore/Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{5F3B4D9E-8663-43A7-A6A0-22959908DEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF30F175-EDF2-411C-B1F6-98F6F0C9EFA0}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{5F3B4D9E-8663-43A7-A6A0-22959908DEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DE6684A-3A28-4AF9-BFCF-DDE7FCB31A69}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{4F61113F-05D2-4FB0-814E-FE2E547F11D4}"/>
+    <workbookView xWindow="45972" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="7" xr2:uid="{4F61113F-05D2-4FB0-814E-FE2E547F11D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Test scenarios" sheetId="1" r:id="rId1"/>
@@ -212,8 +212,200 @@
     <t>Test  A1-7</t>
   </si>
   <si>
-    <r>
-      <t>2 decimal numbers sraers with 0 &amp; dot (</t>
+    <t>Test  A1-6</t>
+  </si>
+  <si>
+    <t>2. Choose the first Number (i.e 12)</t>
+  </si>
+  <si>
+    <t>4. Choose the second Number (i.e 12)</t>
+  </si>
+  <si>
+    <t>Result is 144</t>
+  </si>
+  <si>
+    <t>2. Choose the first Number (i.e 96)</t>
+  </si>
+  <si>
+    <t>4. Choose the second Number (i.e 15.55)</t>
+  </si>
+  <si>
+    <t>This test validates that the multiplication operation is working correctly</t>
+  </si>
+  <si>
+    <t>This test validates that the subtraction operation is working correctly</t>
+  </si>
+  <si>
+    <t>This test validates that the division operation is working correctly</t>
+  </si>
+  <si>
+    <t>Result is 80.34</t>
+  </si>
+  <si>
+    <t>2. Choose the first Number (i.e 85)</t>
+  </si>
+  <si>
+    <t>4. Choose the second Number (i.e 5)</t>
+  </si>
+  <si>
+    <t>Result is 17</t>
+  </si>
+  <si>
+    <r>
+      <t>3. Click multiplication (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3. Click subtraction (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3. Click division (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) button</t>
+    </r>
+  </si>
+  <si>
+    <t>2. input a number (i.e 45687)</t>
+  </si>
+  <si>
+    <t>User is able to input any nmber</t>
+  </si>
+  <si>
+    <r>
+      <t>3. Click Delete  (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) button 2 times</t>
+    </r>
+  </si>
+  <si>
+    <t>Result is 456</t>
+  </si>
+  <si>
+    <t>User is able to select the division operator</t>
+  </si>
+  <si>
+    <t>User is able to select the subtraction operator</t>
+  </si>
+  <si>
+    <t>User is able to select the multiplication operator</t>
+  </si>
+  <si>
+    <t>2 decimal numbers starts with 0 or dot (.) with any operation type [+, -, *, /]</t>
+  </si>
+  <si>
+    <t>2. Choose the first Number (i.e 0.25)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. Choose an operator  (+,-,*,/) button i.e </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <t>4. Choose the second Number (i.e .75)</t>
+  </si>
+  <si>
+    <t>Result is 1</t>
+  </si>
+  <si>
+    <t>prevent users to press F12, right click, Ctrl + Shift + I, Ctrl + Shift + J, Ctrl + U</t>
+  </si>
+  <si>
+    <r>
+      <t>User is able to click 2nd number &amp; get</t>
     </r>
     <r>
       <rPr>
@@ -224,215 +416,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Test  A1-6</t>
-  </si>
-  <si>
-    <t>2. Choose the first Number (i.e 12)</t>
-  </si>
-  <si>
-    <t>4. Choose the second Number (i.e 12)</t>
-  </si>
-  <si>
-    <t>Result is 144</t>
-  </si>
-  <si>
-    <t>2. Choose the first Number (i.e 96)</t>
-  </si>
-  <si>
-    <t>4. Choose the second Number (i.e 15.55)</t>
-  </si>
-  <si>
-    <t>This test validates that the multiplication operation is working correctly</t>
-  </si>
-  <si>
-    <t>This test validates that the subtraction operation is working correctly</t>
-  </si>
-  <si>
-    <t>This test validates that the division operation is working correctly</t>
-  </si>
-  <si>
-    <t>Result is 80.34</t>
-  </si>
-  <si>
-    <t>2. Choose the first Number (i.e 85)</t>
-  </si>
-  <si>
-    <t>4. Choose the second Number (i.e 5)</t>
-  </si>
-  <si>
-    <t>Result is 17</t>
-  </si>
-  <si>
-    <r>
-      <t>3. Click multiplication (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) button</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3. Click subtraction (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) button</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3. Click division (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) button</t>
-    </r>
-  </si>
-  <si>
-    <t>2. input a number (i.e 45687)</t>
-  </si>
-  <si>
-    <t>User is able to input any nmber</t>
-  </si>
-  <si>
-    <r>
-      <t>3. Click Delete  (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) button 2 times</t>
-    </r>
-  </si>
-  <si>
-    <t>Result is 456</t>
-  </si>
-  <si>
-    <t>User is able to select the division operator</t>
-  </si>
-  <si>
-    <t>User is able to select the subtraction operator</t>
-  </si>
-  <si>
-    <t>User is able to select the multiplication operator</t>
-  </si>
-  <si>
-    <t>2 decimal numbers starts with 0 or dot (.) with any operation type [+, -, *, /]</t>
-  </si>
-  <si>
-    <t>2. Choose the first Number (i.e 0.25)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3. Choose an operator  (+,-,*,/) button i.e </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+</t>
-    </r>
-  </si>
-  <si>
-    <t>4. Choose the second Number (i.e .75)</t>
-  </si>
-  <si>
-    <t>Result is 1</t>
-  </si>
-  <si>
-    <t>prevent users to press F12, right click, Ctrl + Shift + I, Ctrl + Shift + J, Ctrl + U</t>
-  </si>
-  <si>
-    <r>
-      <t>User is able to click 2nd number &amp; get</t>
-    </r>
+      <t xml:space="preserve"> 0.75</t>
+    </r>
+  </si>
+  <si>
+    <t>This test validates that the addition operation of 2 decimal numbers starting with 0 or dor (.) is working correctly</t>
+  </si>
+  <si>
+    <t>This test validates that users are able to delete the last added numbers</t>
+  </si>
+  <si>
+    <t>This test validates that users should no be able to use inepect page to inject unwanted js code or HTML</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -442,17 +438,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 0.75</t>
-    </r>
-  </si>
-  <si>
-    <t>This test validates that the addition operation of 2 decimal numbers starting with 0 or dor (.) is working correctly</t>
-  </si>
-  <si>
-    <t>This test validates that users are able to delete the last added numbers</t>
-  </si>
-  <si>
-    <t>This test validates that users should no be able to use inepect page to inject unwanted js code or HTML</t>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: this test can be also tested from the keyboard numbers as well</t>
+    </r>
   </si>
   <si>
     <r>
@@ -474,10 +471,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: this test can be also tested from the keyboard numbers as well</t>
-    </r>
-  </si>
-  <si>
+      <t>: this test can be also tested from the keyboard "</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -487,7 +482,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note</t>
+      <t>backspace</t>
     </r>
     <r>
       <rPr>
@@ -497,8 +492,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: this test can be also tested from the keyboard "</t>
-    </r>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -508,7 +505,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>backspace</t>
+      <t>Note</t>
     </r>
     <r>
       <rPr>
@@ -518,10 +515,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
+      <t>: this test can be also tested from the keyboard for both numbers &amp; operators "</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -531,7 +526,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note</t>
+      <t>/</t>
     </r>
     <r>
       <rPr>
@@ -541,8 +536,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: this test can be also tested from the keyboard for both numbers &amp; operators "</t>
-    </r>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -552,7 +549,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/</t>
+      <t>Note</t>
     </r>
     <r>
       <rPr>
@@ -562,10 +559,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
+      <t>: this test can be also tested from the keyboard for both numbers &amp; operators "</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -575,7 +570,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note</t>
+      <t>*</t>
     </r>
     <r>
       <rPr>
@@ -585,8 +580,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: this test can be also tested from the keyboard for both numbers &amp; operators "</t>
-    </r>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -596,7 +593,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>*</t>
+      <t>Note</t>
     </r>
     <r>
       <rPr>
@@ -606,10 +603,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
+      <t>: this test can be also tested from the keyboard for both numbers &amp; operators "</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -619,7 +614,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note</t>
+      <t>-</t>
     </r>
     <r>
       <rPr>
@@ -629,8 +624,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: this test can be also tested from the keyboard for both numbers &amp; operators "</t>
-    </r>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -640,7 +637,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>-</t>
+      <t>Note</t>
     </r>
     <r>
       <rPr>
@@ -650,10 +647,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
+      <t>: this test can be also tested from the keyboard for both numbers &amp; operators "</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -663,7 +658,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note</t>
+      <t>+</t>
     </r>
     <r>
       <rPr>
@@ -673,7 +668,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: this test can be also tested from the keyboard for both numbers &amp; operators "</t>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2 decimal numbers srarts with 0 &amp; dot (</t>
     </r>
     <r>
       <rPr>
@@ -684,7 +684,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>+</t>
+      <t>.</t>
     </r>
     <r>
       <rPr>
@@ -694,7 +694,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"</t>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -1048,7 +1048,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1069,44 +1069,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1128,15 +1104,42 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1147,9 +1150,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1167,6 +1167,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1468,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A6B141-0015-4B6D-B75D-0FA76526973F}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1531,7 +1535,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.75">
@@ -1553,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B082AAAC-6FF9-4B39-B966-71546B5DCB4B}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1598,108 +1602,108 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="73.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
+      <c r="I6" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="19"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="14"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="12" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1766,108 +1770,108 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="73.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
+      <c r="I6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="27"/>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B8" s="27"/>
+      <c r="C8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B9" s="27"/>
+      <c r="C9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-    </row>
-    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="14"/>
-      <c r="C9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="33" t="s">
+      <c r="E9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="12" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1934,108 +1938,108 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="73.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
+      <c r="I6" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="27"/>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B8" s="27"/>
+      <c r="C8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B9" s="27"/>
+      <c r="C9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-    </row>
-    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="14"/>
-      <c r="C9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="E10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="12" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2102,108 +2106,108 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="73.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
+      <c r="I6" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="27"/>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B8" s="27"/>
+      <c r="C8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B9" s="27"/>
+      <c r="C9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-    </row>
-    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="14"/>
-      <c r="C9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="33" t="s">
+      <c r="E9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="12" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2226,7 +2230,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G5" sqref="G5:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2270,100 +2274,100 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="73.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="14"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
+      <c r="I6" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="27"/>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B8" s="27"/>
+      <c r="C8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B9" s="27"/>
+      <c r="C9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-    </row>
-    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="14"/>
-      <c r="C9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="29" t="s">
+      <c r="E9" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="12" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2404,10 +2408,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
@@ -2432,108 +2436,108 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="73.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
+      <c r="I6" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="27"/>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="I6" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-    </row>
-    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="E7" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B8" s="27"/>
+      <c r="C8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B9" s="27"/>
+      <c r="C9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="14"/>
-      <c r="C9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="33" t="s">
+      <c r="E9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="12" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2555,8 +2559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432F90F4-27E3-4604-AFD4-962DA4DE88F6}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2575,7 +2579,7 @@
         <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
@@ -2600,103 +2604,103 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="29.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" ht="73.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="14"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="19"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="14"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="14"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7" ht="74.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="12" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="19" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>